<commit_message>
Renamed the import statement of ExcelDataTest Handler to ExcelHandler in these classes
</commit_message>
<xml_diff>
--- a/filesToUpload/EmailTemplate-MLC.xlsx
+++ b/filesToUpload/EmailTemplate-MLC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05961A2-0B36-4299-AE7D-4C62805419CB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8F8D7D-2FA9-4FE3-AA97-F6C5393DD0F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Email Template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>E-mail Address</t>
   </si>
@@ -53,16 +53,19 @@
     <t>Needed for multi-location campaign type</t>
   </si>
   <si>
-    <t>akram.1wasi@gmail.com</t>
+    <t>wasimakramb325@gmail.com</t>
+  </si>
+  <si>
+    <t>wasim</t>
+  </si>
+  <si>
+    <t>akram</t>
   </si>
   <si>
     <t>wakram@dacgroup.com</t>
   </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>Wasim</t>
   </si>
   <si>
     <t>Akram</t>
@@ -500,12 +503,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
@@ -530,10 +533,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>9000045062</v>
@@ -541,16 +544,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>9990038503</v>
+        <v>9990038502</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,8 +561,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{10A7454F-90EC-4E2A-B408-14AA6B391712}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{7778041F-B9D0-478B-A1EC-B0C438F2BEB2}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0EC36D9E-CB99-4353-881A-50869C4DDE52}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7F874732-BF74-4659-BC2D-53369670D553}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -570,7 +573,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>